<commit_message>
Open & extract work items, logout
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19665" windowHeight="6405" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7875"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -36,36 +36,36 @@
     <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
   </si>
   <si>
-    <t>AcmeCredential</t>
-  </si>
-  <si>
-    <t>AcmeCredential_REFramework</t>
+    <t>logF_BusinessProcessName</t>
+  </si>
+  <si>
+    <t>Framework</t>
+  </si>
+  <si>
+    <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
+  </si>
+  <si>
+    <t>System1_URL</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/</t>
+  </si>
+  <si>
+    <t>SHA1_Online_URL</t>
+  </si>
+  <si>
+    <t>http://www.sha1-online.com/</t>
+  </si>
+  <si>
+    <t>System1_Credential</t>
+  </si>
+  <si>
+    <t>in_System1Credential</t>
   </si>
   <si>
     <t>Credential used to login into UiDemo</t>
   </si>
   <si>
-    <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
-  </si>
-  <si>
-    <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
-  </si>
-  <si>
-    <t>System1_URL</t>
-  </si>
-  <si>
-    <t>https://acme-test.uipath.com/</t>
-  </si>
-  <si>
-    <t>SHA1_Online_URL</t>
-  </si>
-  <si>
-    <t>http://www.sha1-online.com/</t>
-  </si>
-  <si>
     <t>MaxRetryNumber</t>
   </si>
   <si>
@@ -186,7 +186,10 @@
     <t>Description (Assets will always overwrite other config)</t>
   </si>
   <si>
-    <t>is_Credential_Acme</t>
+    <t>in_Credential</t>
+  </si>
+  <si>
+    <t>Credential to get assest from orcestrator</t>
   </si>
 </sst>
 </file>
@@ -194,10 +197,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -217,13 +220,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -249,13 +245,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -322,14 +311,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -351,6 +340,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -360,6 +356,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -374,25 +377,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -410,7 +413,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -422,43 +461,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -476,37 +491,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -524,13 +527,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -548,13 +551,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -668,148 +671,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1139,8 +1142,8 @@
   <sheetPr/>
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -1196,45 +1199,45 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1" spans="1:3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
+    <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="14.25" customHeight="1" spans="1:3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1" spans="1:2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1" spans="1:2">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25" customHeight="1" spans="1:3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1"/>
     <row r="8" ht="14.25" customHeight="1"/>
     <row r="9" ht="14.25" customHeight="1"/>
     <row r="10" ht="14.25" customHeight="1"/>
@@ -2240,8 +2243,8 @@
   <sheetPr/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -3457,7 +3460,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -3499,12 +3502,15 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1" spans="1:2">
+    <row r="2" ht="14.25" customHeight="1" spans="1:3">
       <c r="A2" t="s">
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Completed code, testing pending
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -197,10 +197,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -449,12 +449,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -534,6 +528,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -674,12 +674,12 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -743,7 +743,7 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
@@ -758,61 +758,61 @@
     <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1143,7 +1143,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>

</xml_diff>